<commit_message>
Add TENDERS ISIC with AS-39 and AS-40 submarine tenders
- Add TENDERS as new ISIC under CSP
- Add USS Emory S. Land (AS-39) and USS Frank Cable (AS-40)
- Update normalizeBoatName regex to handle AS-XX format
- Regenerate test data files (now 60 vessels total)
</commit_message>
<xml_diff>
--- a/test-data/TAM-Overdue-Test.xlsx
+++ b/test-data/TAM-Overdue-Test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,7 +418,7 @@
         <v>SSN-775</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -429,10 +429,10 @@
         <v>SSN-776</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -440,10 +440,10 @@
         <v>SSN-777</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -451,10 +451,10 @@
         <v>SSN-786</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -462,7 +462,7 @@
         <v>SSN-792</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -473,10 +473,10 @@
         <v>SSN-794</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -484,10 +484,10 @@
         <v>SSN-762</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -495,10 +495,10 @@
         <v>SSN-763</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -506,10 +506,10 @@
         <v>SSN-766</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -528,10 +528,10 @@
         <v>SSN-772</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -539,10 +539,10 @@
         <v>SSN-773</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -550,10 +550,10 @@
         <v>SSN-752</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -561,10 +561,10 @@
         <v>SSN-754</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -572,10 +572,10 @@
         <v>SSN-758</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -583,10 +583,10 @@
         <v>SSN-767</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -594,7 +594,7 @@
         <v>SSN-722</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -605,7 +605,7 @@
         <v>SSN-759</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -616,7 +616,7 @@
         <v>SSN-760</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -627,10 +627,10 @@
         <v>SSN-761</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -638,10 +638,10 @@
         <v>SSN-783</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -660,10 +660,10 @@
         <v>SSBN-731</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -671,10 +671,10 @@
         <v>SSBN-733</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -682,10 +682,10 @@
         <v>SSBN-739</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -693,7 +693,7 @@
         <v>SSBN-741</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -704,10 +704,10 @@
         <v>SSBN-743</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -729,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -748,10 +748,10 @@
         <v>SSBN-737</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -759,10 +759,10 @@
         <v>SSN-21</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -770,10 +770,10 @@
         <v>SSN-22</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -781,18 +781,18 @@
         <v>SSN-23</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>SSN-774</v>
+        <v>AS-39</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -800,106 +800,106 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>SSN-778</v>
+        <v>AS-40</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>SSN-779</v>
+        <v>SSN-774</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>SSN-780</v>
+        <v>SSN-778</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>SSN-781</v>
+        <v>SSN-779</v>
       </c>
       <c r="B40">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>SSN-795</v>
+        <v>SSN-780</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>SSN-753</v>
+        <v>SSN-781</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>SSN-756</v>
+        <v>SSN-795</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>SSN-764</v>
+        <v>SSN-753</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>SSN-765</v>
+        <v>SSN-756</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>SSN-791</v>
+        <v>SSN-764</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -910,76 +910,76 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>SSN-793</v>
+        <v>SSN-765</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>SSN-750</v>
+        <v>SSN-791</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>SSN-751</v>
+        <v>SSN-793</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>SSN-768</v>
+        <v>SSN-750</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>SSN-769</v>
+        <v>SSN-751</v>
       </c>
       <c r="B51">
         <v>3</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>SSN-785</v>
+        <v>SSN-768</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>SSGN-728</v>
+        <v>SSN-769</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -987,18 +987,18 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>SSGN-729</v>
+        <v>SSN-785</v>
       </c>
       <c r="B54">
         <v>3</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>SSBN-734</v>
+        <v>SSGN-728</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -1009,51 +1009,73 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>SSBN-736</v>
+        <v>SSGN-729</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>SSBN-738</v>
+        <v>SSBN-734</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>SSBN-740</v>
+        <v>SSBN-736</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
+        <v>SSBN-738</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>SSBN-740</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
         <v>SSBN-742</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59">
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C59"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix VRAM test data column names to match schema
- 'RA CRIT' -> 'RA Critical'
- 'RA HIGH' -> 'RA High'
- 'Scan %' -> 'Percent Scanned'

ESS data already includes Assets column correctly.
</commit_message>
<xml_diff>
--- a/test-data/TAM-Overdue-Test.xlsx
+++ b/test-data/TAM-Overdue-Test.xlsx
@@ -421,7 +421,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -429,10 +429,10 @@
         <v>SSN-776</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -440,10 +440,10 @@
         <v>SSN-777</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -451,10 +451,10 @@
         <v>SSN-786</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -465,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -473,7 +473,7 @@
         <v>SSN-794</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -484,10 +484,10 @@
         <v>SSN-762</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -495,10 +495,10 @@
         <v>SSN-763</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -506,7 +506,7 @@
         <v>SSN-766</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -517,10 +517,10 @@
         <v>SSN-771</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -539,10 +539,10 @@
         <v>SSN-773</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -550,7 +550,7 @@
         <v>SSN-752</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -561,10 +561,10 @@
         <v>SSN-754</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -572,10 +572,10 @@
         <v>SSN-758</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -583,7 +583,7 @@
         <v>SSN-767</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -594,10 +594,10 @@
         <v>SSN-722</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -605,7 +605,7 @@
         <v>SSN-759</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -616,10 +616,10 @@
         <v>SSN-760</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -638,10 +638,10 @@
         <v>SSN-783</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -649,7 +649,7 @@
         <v>SSBN-730</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -660,7 +660,7 @@
         <v>SSBN-731</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -671,10 +671,10 @@
         <v>SSBN-733</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -682,10 +682,10 @@
         <v>SSBN-739</v>
       </c>
       <c r="B26">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -693,7 +693,7 @@
         <v>SSBN-741</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -704,7 +704,7 @@
         <v>SSBN-743</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -715,10 +715,10 @@
         <v>SSGN-726</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -726,7 +726,7 @@
         <v>SSGN-727</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -737,10 +737,10 @@
         <v>SSBN-735</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -748,10 +748,10 @@
         <v>SSBN-737</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -759,10 +759,10 @@
         <v>SSN-21</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -770,10 +770,10 @@
         <v>SSN-22</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -781,10 +781,10 @@
         <v>SSN-23</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -795,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -814,10 +814,10 @@
         <v>SSN-774</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -825,10 +825,10 @@
         <v>SSN-778</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -836,10 +836,10 @@
         <v>SSN-779</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -869,10 +869,10 @@
         <v>SSN-795</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -880,7 +880,7 @@
         <v>SSN-753</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -891,10 +891,10 @@
         <v>SSN-756</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -902,10 +902,10 @@
         <v>SSN-764</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -913,10 +913,10 @@
         <v>SSN-765</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -927,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -946,10 +946,10 @@
         <v>SSN-750</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -957,10 +957,10 @@
         <v>SSN-751</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -968,10 +968,10 @@
         <v>SSN-768</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
@@ -979,10 +979,10 @@
         <v>SSN-769</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -990,10 +990,10 @@
         <v>SSN-785</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1001,10 +1001,10 @@
         <v>SSGN-728</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -1012,10 +1012,10 @@
         <v>SSGN-729</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1023,10 +1023,10 @@
         <v>SSBN-734</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
@@ -1034,10 +1034,10 @@
         <v>SSBN-736</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -1048,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1056,10 +1056,10 @@
         <v>SSBN-740</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1067,10 +1067,10 @@
         <v>SSBN-742</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix test data column names to match schema
VRAM:
- Added missing 'Scan Exempt' column

ESS:
- 'ISIC' -> 'ISICs' (match schema)
- 'Assets' -> 'Asset Count' (match schema)
</commit_message>
<xml_diff>
--- a/test-data/TAM-Overdue-Test.xlsx
+++ b/test-data/TAM-Overdue-Test.xlsx
@@ -421,7 +421,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -429,10 +429,10 @@
         <v>SSN-776</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -440,10 +440,10 @@
         <v>SSN-777</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -451,7 +451,7 @@
         <v>SSN-786</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -462,10 +462,10 @@
         <v>SSN-792</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -473,10 +473,10 @@
         <v>SSN-794</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -484,7 +484,7 @@
         <v>SSN-762</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>SSN-763</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -506,10 +506,10 @@
         <v>SSN-766</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -517,10 +517,10 @@
         <v>SSN-771</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -528,7 +528,7 @@
         <v>SSN-772</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -539,10 +539,10 @@
         <v>SSN-773</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -550,7 +550,7 @@
         <v>SSN-752</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -561,10 +561,10 @@
         <v>SSN-754</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -572,7 +572,7 @@
         <v>SSN-758</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -583,10 +583,10 @@
         <v>SSN-767</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -594,10 +594,10 @@
         <v>SSN-722</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -605,10 +605,10 @@
         <v>SSN-759</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -616,10 +616,10 @@
         <v>SSN-760</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -638,10 +638,10 @@
         <v>SSN-783</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -649,7 +649,7 @@
         <v>SSBN-730</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -682,10 +682,10 @@
         <v>SSBN-739</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -704,10 +704,10 @@
         <v>SSBN-743</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -715,10 +715,10 @@
         <v>SSGN-726</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -726,7 +726,7 @@
         <v>SSGN-727</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -737,10 +737,10 @@
         <v>SSBN-735</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -748,10 +748,10 @@
         <v>SSBN-737</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -759,10 +759,10 @@
         <v>SSN-21</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -770,10 +770,10 @@
         <v>SSN-22</v>
       </c>
       <c r="B34">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -781,7 +781,7 @@
         <v>SSN-23</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -792,10 +792,10 @@
         <v>AS-39</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -803,10 +803,10 @@
         <v>AS-40</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
@@ -814,10 +814,10 @@
         <v>SSN-774</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -828,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -858,10 +858,10 @@
         <v>SSN-781</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -880,10 +880,10 @@
         <v>SSN-753</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -891,10 +891,10 @@
         <v>SSN-756</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -902,10 +902,10 @@
         <v>SSN-764</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -916,7 +916,7 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -924,10 +924,10 @@
         <v>SSN-791</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -935,10 +935,10 @@
         <v>SSN-793</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -946,10 +946,10 @@
         <v>SSN-750</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -957,10 +957,10 @@
         <v>SSN-751</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -968,10 +968,10 @@
         <v>SSN-768</v>
       </c>
       <c r="B52">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -979,10 +979,10 @@
         <v>SSN-769</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -990,10 +990,10 @@
         <v>SSN-785</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1001,10 +1001,10 @@
         <v>SSGN-728</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -1012,7 +1012,7 @@
         <v>SSGN-729</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1023,10 +1023,10 @@
         <v>SSBN-734</v>
       </c>
       <c r="B57">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -1034,7 +1034,7 @@
         <v>SSBN-736</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -1045,10 +1045,10 @@
         <v>SSBN-738</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1056,10 +1056,10 @@
         <v>SSBN-740</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1067,10 +1067,10 @@
         <v>SSBN-742</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>